<commit_message>
plans are changing dynamically
</commit_message>
<xml_diff>
--- a/Weekly Tasks Folder/Насибова Севиль & Мазитова Лилия.xlsx
+++ b/Weekly Tasks Folder/Насибова Севиль & Мазитова Лилия.xlsx
@@ -56,27 +56,6 @@
     <t>Воскресенье</t>
   </si>
   <si>
-    <t>Урок№1-2</t>
-  </si>
-  <si>
-    <t>Урок№3-4</t>
-  </si>
-  <si>
-    <t>Урок№5-6</t>
-  </si>
-  <si>
-    <t>Урок№7-8</t>
-  </si>
-  <si>
-    <t>Урок№9</t>
-  </si>
-  <si>
-    <t>Урок№10</t>
-  </si>
-  <si>
-    <t>Урок№11</t>
-  </si>
-  <si>
     <t>Ссылка</t>
   </si>
   <si>
@@ -90,6 +69,27 @@
   </si>
   <si>
     <t>дата - 20.02.2016</t>
+  </si>
+  <si>
+    <t>Урок№1</t>
+  </si>
+  <si>
+    <t>Урок№2</t>
+  </si>
+  <si>
+    <t>Урок№3</t>
+  </si>
+  <si>
+    <t>Урок№4</t>
+  </si>
+  <si>
+    <t>Урок№5</t>
+  </si>
+  <si>
+    <t>Урок№6</t>
+  </si>
+  <si>
+    <t>Урок№7</t>
   </si>
 </sst>
 </file>
@@ -188,35 +188,63 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -494,7 +522,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,187 +537,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="4"/>
+      <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
+      <c r="A5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="A6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="A9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="A10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
+      <c r="A12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="1"/>
+      <c r="H13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="8"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="1"/>
+      <c r="H14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="1"/>
+      <c r="H15" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="A7:B7"/>
@@ -698,12 +732,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A12:I12"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A12" r:id="rId1"/>

</xml_diff>